<commit_message>
added notebooks to tunne the growth rates of certain sectors
</commit_message>
<xml_diff>
--- a/ssp_modeling/scenario_mapping/ssp_morocco_transformation_cw.xlsx
+++ b/ssp_modeling/scenario_mapping/ssp_morocco_transformation_cw.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10921"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Documents/sisepuede_modeling/ssp_egypt/ssp_modeling/scenario_mapping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Documents/sisepuede_modeling/ssp_morocco/ssp_modeling/scenario_mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0992AD1-8568-A648-AC02-91DA757AC63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDB247D-01BB-B94C-BDF8-E60C36F7A3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="500" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="yaml" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">main!$A$1:$N$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">main!$A$1:$M$62</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">yaml!$A$1:$D$62</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="407">
   <si>
     <t>subsector</t>
   </si>
@@ -662,12 +662,6 @@
   </si>
   <si>
     <t>default_magnitude</t>
-  </si>
-  <si>
-    <t>strategy_NDC</t>
-  </si>
-  <si>
-    <t>strategy_NZ</t>
   </si>
   <si>
     <t>AFOLU</t>
@@ -1308,6 +1302,9 @@
   </si>
   <si>
     <t>magnitude_description</t>
+  </si>
+  <si>
+    <t>strategy_LEP</t>
   </si>
 </sst>
 </file>
@@ -1915,11 +1912,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:R65"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1934,14 +1931,14 @@
     <col min="9" max="10" width="35" style="4" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="31.5" style="39" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.83203125" style="38" customWidth="1"/>
-    <col min="13" max="14" width="20.5" style="40" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5" style="41" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5" style="42" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5" style="40" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5" style="43" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5" style="40" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" style="41" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5" style="42" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" style="40" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5" style="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>203</v>
       </c>
@@ -1961,16 +1958,16 @@
         <v>205</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>405</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>407</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>207</v>
@@ -1979,19 +1976,16 @@
         <v>206</v>
       </c>
       <c r="M1" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+    </row>
+    <row r="2" spans="1:17" s="4" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>208</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-    </row>
-    <row r="2" spans="1:18" s="4" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>210</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>4</v>
@@ -2003,10 +1997,10 @@
         <v>6</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -2021,17 +2015,14 @@
       <c r="M2" s="16">
         <v>1</v>
       </c>
-      <c r="N2" s="16">
-        <v>1</v>
-      </c>
+      <c r="N2" s="10"/>
       <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
+      <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-    </row>
-    <row r="3" spans="1:18" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B3" s="45" t="s">
         <v>4</v>
@@ -2043,10 +2034,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -2059,17 +2050,14 @@
         <v>12</v>
       </c>
       <c r="M3" s="16"/>
-      <c r="N3" s="16">
-        <v>1</v>
-      </c>
+      <c r="N3" s="10"/>
       <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
+      <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-    </row>
-    <row r="4" spans="1:18" s="4" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>4</v>
@@ -2081,10 +2069,10 @@
         <v>12</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
@@ -2097,17 +2085,14 @@
         <v>12</v>
       </c>
       <c r="M4" s="16"/>
-      <c r="N4" s="16">
-        <v>1</v>
-      </c>
+      <c r="N4" s="10"/>
       <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-    </row>
-    <row r="5" spans="1:18" s="4" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>4</v>
@@ -2119,35 +2104,30 @@
         <v>15</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="20" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="L5" s="13">
         <v>12</v>
       </c>
-      <c r="M5" s="16">
-        <v>1</v>
-      </c>
-      <c r="N5" s="16">
-        <v>1</v>
-      </c>
+      <c r="M5" s="16"/>
+      <c r="N5" s="10"/>
       <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
+      <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-    </row>
-    <row r="6" spans="1:18" s="4" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B6" s="26" t="s">
         <v>4</v>
@@ -2159,18 +2139,18 @@
         <v>18</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="K6" s="18">
         <v>0.2</v>
@@ -2178,20 +2158,15 @@
       <c r="L6" s="13">
         <v>12</v>
       </c>
-      <c r="M6" s="16">
-        <v>1</v>
-      </c>
-      <c r="N6" s="16">
-        <v>1</v>
-      </c>
+      <c r="M6" s="16"/>
+      <c r="N6" s="10"/>
       <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
+      <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-    </row>
-    <row r="7" spans="1:18" s="4" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>20</v>
@@ -2203,10 +2178,10 @@
         <v>22</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -2218,18 +2193,17 @@
       <c r="L7" s="13">
         <v>12</v>
       </c>
-      <c r="M7" s="16"/>
-      <c r="N7" s="46">
-        <v>0.1</v>
-      </c>
+      <c r="M7" s="46">
+        <v>1</v>
+      </c>
+      <c r="N7" s="10"/>
       <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-    </row>
-    <row r="8" spans="1:18" s="4" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>24</v>
@@ -2241,39 +2215,36 @@
         <v>26</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="K8" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="J8" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>231</v>
-      </c>
       <c r="L8" s="13">
         <v>12</v>
       </c>
-      <c r="M8" s="16">
-        <v>1</v>
-      </c>
-      <c r="N8" s="16">
-        <v>1</v>
-      </c>
+      <c r="M8" s="46">
+        <v>1</v>
+      </c>
+      <c r="N8" s="10"/>
       <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-    </row>
-    <row r="9" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B9" s="26" t="s">
         <v>24</v>
@@ -2285,18 +2256,18 @@
         <v>29</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K9" s="18">
         <v>0.95</v>
@@ -2304,20 +2275,17 @@
       <c r="L9" s="13">
         <v>12</v>
       </c>
-      <c r="M9" s="16">
-        <v>1</v>
-      </c>
-      <c r="N9" s="16">
-        <v>1</v>
-      </c>
+      <c r="M9" s="46">
+        <v>1</v>
+      </c>
+      <c r="N9" s="10"/>
       <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
+      <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-    </row>
-    <row r="10" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>24</v>
@@ -2329,18 +2297,18 @@
         <v>32</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K10" s="18">
         <v>0.95</v>
@@ -2348,20 +2316,17 @@
       <c r="L10" s="13">
         <v>12</v>
       </c>
-      <c r="M10" s="16">
-        <v>1</v>
-      </c>
-      <c r="N10" s="16">
-        <v>1</v>
-      </c>
+      <c r="M10" s="46">
+        <v>1</v>
+      </c>
+      <c r="N10" s="10"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
+      <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-    </row>
-    <row r="11" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>34</v>
@@ -2373,10 +2338,10 @@
         <v>36</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -2388,18 +2353,17 @@
       <c r="L11" s="13">
         <v>12</v>
       </c>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16">
-        <v>1</v>
-      </c>
+      <c r="M11" s="46">
+        <v>1</v>
+      </c>
+      <c r="N11" s="10"/>
       <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
+      <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-    </row>
-    <row r="12" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>34</v>
@@ -2411,10 +2375,10 @@
         <v>39</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
@@ -2426,18 +2390,17 @@
       <c r="L12" s="13">
         <v>12</v>
       </c>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16">
-        <v>1</v>
-      </c>
+      <c r="M12" s="46">
+        <v>1</v>
+      </c>
+      <c r="N12" s="10"/>
       <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
+      <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-    </row>
-    <row r="13" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B13" s="26" t="s">
         <v>41</v>
@@ -2449,18 +2412,18 @@
         <v>43</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="K13" s="20">
         <v>0.3</v>
@@ -2468,20 +2431,17 @@
       <c r="L13" s="13">
         <v>12</v>
       </c>
-      <c r="M13" s="16">
-        <v>1</v>
-      </c>
-      <c r="N13" s="16">
-        <v>1</v>
-      </c>
+      <c r="M13" s="46">
+        <v>1</v>
+      </c>
+      <c r="N13" s="10"/>
       <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
+      <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-    </row>
-    <row r="14" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>41</v>
@@ -2493,18 +2453,18 @@
         <v>46</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K14" s="20">
         <v>0.4</v>
@@ -2512,20 +2472,17 @@
       <c r="L14" s="13">
         <v>12</v>
       </c>
-      <c r="M14" s="16">
-        <v>0.6</v>
-      </c>
-      <c r="N14" s="16">
-        <v>1</v>
-      </c>
+      <c r="M14" s="46">
+        <v>1</v>
+      </c>
+      <c r="N14" s="10"/>
       <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
+      <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-    </row>
-    <row r="15" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>41</v>
@@ -2537,31 +2494,30 @@
         <v>49</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="L15" s="13">
         <v>12</v>
       </c>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16">
-        <v>1</v>
-      </c>
+      <c r="M15" s="46">
+        <v>1</v>
+      </c>
+      <c r="N15" s="10"/>
       <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
+      <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-    </row>
-    <row r="16" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>51</v>
       </c>
@@ -2575,18 +2531,18 @@
         <v>53</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K16" s="15">
         <v>0.5</v>
@@ -2594,18 +2550,15 @@
       <c r="L16" s="13">
         <v>12</v>
       </c>
-      <c r="M16" s="16">
-        <v>1</v>
-      </c>
-      <c r="N16" s="16">
-        <v>1</v>
-      </c>
+      <c r="M16" s="46">
+        <v>1</v>
+      </c>
+      <c r="N16" s="10"/>
       <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
+      <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-    </row>
-    <row r="17" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>51</v>
       </c>
@@ -2619,18 +2572,18 @@
         <v>56</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="K17" s="18">
         <v>0.3</v>
@@ -2638,18 +2591,15 @@
       <c r="L17" s="13">
         <v>12</v>
       </c>
-      <c r="M17" s="16">
-        <v>1</v>
-      </c>
-      <c r="N17" s="16">
-        <v>1</v>
-      </c>
+      <c r="M17" s="46">
+        <v>1</v>
+      </c>
+      <c r="N17" s="10"/>
       <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
+      <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-    </row>
-    <row r="18" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>51</v>
       </c>
@@ -2663,18 +2613,18 @@
         <v>59</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="K18" s="15">
         <v>0.1</v>
@@ -2682,18 +2632,15 @@
       <c r="L18" s="13">
         <v>12</v>
       </c>
-      <c r="M18" s="16">
-        <v>1</v>
-      </c>
-      <c r="N18" s="16">
-        <v>1</v>
-      </c>
+      <c r="M18" s="46">
+        <v>1</v>
+      </c>
+      <c r="N18" s="10"/>
       <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
+      <c r="P18" s="11"/>
       <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-    </row>
-    <row r="19" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>51</v>
       </c>
@@ -2707,10 +2654,10 @@
         <v>62</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
@@ -2722,16 +2669,15 @@
       <c r="L19" s="13">
         <v>12</v>
       </c>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16">
-        <v>1</v>
-      </c>
+      <c r="M19" s="46">
+        <v>1</v>
+      </c>
+      <c r="N19" s="10"/>
       <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-    </row>
-    <row r="20" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>51</v>
       </c>
@@ -2745,10 +2691,10 @@
         <v>65</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
@@ -2760,16 +2706,15 @@
       <c r="L20" s="13">
         <v>12</v>
       </c>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16">
-        <v>1</v>
-      </c>
+      <c r="M20" s="46">
+        <v>1</v>
+      </c>
+      <c r="N20" s="10"/>
       <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
+      <c r="P20" s="11"/>
       <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-    </row>
-    <row r="21" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>51</v>
       </c>
@@ -2783,10 +2728,10 @@
         <v>68</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
@@ -2798,18 +2743,17 @@
       <c r="L21" s="13">
         <v>12</v>
       </c>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16">
-        <v>1</v>
-      </c>
+      <c r="M21" s="46">
+        <v>1</v>
+      </c>
+      <c r="N21" s="10"/>
       <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
+      <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-    </row>
-    <row r="22" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B22" s="26" t="s">
         <v>70</v>
@@ -2821,18 +2765,18 @@
         <v>72</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="26" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J22" s="26" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K22" s="15">
         <v>0.999</v>
@@ -2840,20 +2784,17 @@
       <c r="L22" s="13">
         <v>12</v>
       </c>
-      <c r="M22" s="16">
-        <v>0.89</v>
-      </c>
-      <c r="N22" s="16">
-        <v>1</v>
-      </c>
+      <c r="M22" s="46">
+        <v>1</v>
+      </c>
+      <c r="N22" s="10"/>
       <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
+      <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-    </row>
-    <row r="23" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B23" s="26" t="s">
         <v>70</v>
@@ -2865,18 +2806,18 @@
         <v>75</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J23" s="27" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="K23" s="18">
         <v>0.95</v>
@@ -2884,16 +2825,17 @@
       <c r="L23" s="13">
         <v>12</v>
       </c>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
+      <c r="M23" s="46">
+        <v>1</v>
+      </c>
+      <c r="N23" s="10"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
+      <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-    </row>
-    <row r="24" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>70</v>
@@ -2905,18 +2847,18 @@
         <v>78</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
       <c r="I24" s="26" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J24" s="26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K24" s="15">
         <v>0.2</v>
@@ -2924,20 +2866,17 @@
       <c r="L24" s="13">
         <v>12</v>
       </c>
-      <c r="M24" s="16">
-        <v>2</v>
-      </c>
-      <c r="N24" s="16">
-        <v>2</v>
-      </c>
+      <c r="M24" s="46">
+        <v>1</v>
+      </c>
+      <c r="N24" s="10"/>
       <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
+      <c r="P24" s="11"/>
       <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-    </row>
-    <row r="25" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B25" s="26" t="s">
         <v>70</v>
@@ -2949,18 +2888,18 @@
         <v>81</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K25" s="18">
         <v>0.1</v>
@@ -2968,16 +2907,17 @@
       <c r="L25" s="13">
         <v>12</v>
       </c>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
+      <c r="M25" s="46">
+        <v>1</v>
+      </c>
+      <c r="N25" s="10"/>
       <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
+      <c r="P25" s="11"/>
       <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-    </row>
-    <row r="26" spans="1:18" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:17" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B26" s="26" t="s">
         <v>83</v>
@@ -2989,10 +2929,10 @@
         <v>85</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
@@ -3004,20 +2944,17 @@
       <c r="L26" s="13">
         <v>12</v>
       </c>
-      <c r="M26" s="16">
-        <v>1.05</v>
-      </c>
-      <c r="N26" s="16">
-        <v>1.05</v>
-      </c>
+      <c r="M26" s="46">
+        <v>1</v>
+      </c>
+      <c r="N26" s="28"/>
       <c r="O26" s="28"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="29"/>
-      <c r="R26" s="30"/>
-    </row>
-    <row r="27" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P26" s="29"/>
+      <c r="Q26" s="30"/>
+    </row>
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B27" s="26" t="s">
         <v>83</v>
@@ -3029,35 +2966,32 @@
         <v>88</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="18" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="L27" s="13">
         <v>12</v>
       </c>
-      <c r="M27" s="16">
-        <v>1</v>
-      </c>
-      <c r="N27" s="16">
-        <v>1</v>
-      </c>
+      <c r="M27" s="46">
+        <v>1</v>
+      </c>
+      <c r="N27" s="10"/>
       <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
+      <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-    </row>
-    <row r="28" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B28" s="26" t="s">
         <v>83</v>
@@ -3069,35 +3003,32 @@
         <v>91</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="18" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="L28" s="13">
         <v>12</v>
       </c>
-      <c r="M28" s="16">
-        <v>1</v>
-      </c>
-      <c r="N28" s="16">
-        <v>1</v>
-      </c>
+      <c r="M28" s="46">
+        <v>1</v>
+      </c>
+      <c r="N28" s="10"/>
       <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
+      <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
-    </row>
-    <row r="29" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B29" s="26" t="s">
         <v>83</v>
@@ -3109,35 +3040,32 @@
         <v>94</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="18" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="L29" s="13">
         <v>12</v>
       </c>
-      <c r="M29" s="16">
-        <v>1</v>
-      </c>
-      <c r="N29" s="16">
-        <v>1</v>
-      </c>
+      <c r="M29" s="46">
+        <v>1</v>
+      </c>
+      <c r="N29" s="10"/>
       <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
+      <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
-      <c r="R29" s="11"/>
-    </row>
-    <row r="30" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B30" s="26" t="s">
         <v>96</v>
@@ -3149,33 +3077,32 @@
         <v>98</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="15" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L30" s="13">
         <v>12</v>
       </c>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16">
-        <v>1</v>
-      </c>
+      <c r="M30" s="46">
+        <v>1</v>
+      </c>
+      <c r="N30" s="10"/>
       <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
+      <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-    </row>
-    <row r="31" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B31" s="26" t="s">
         <v>96</v>
@@ -3187,10 +3114,10 @@
         <v>101</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
@@ -3202,18 +3129,17 @@
       <c r="L31" s="13">
         <v>12</v>
       </c>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16">
-        <v>1</v>
-      </c>
+      <c r="M31" s="46">
+        <v>1</v>
+      </c>
+      <c r="N31" s="10"/>
       <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
+      <c r="P31" s="11"/>
       <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-    </row>
-    <row r="32" spans="1:18" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:17" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B32" s="26" t="s">
         <v>96</v>
@@ -3225,18 +3151,18 @@
         <v>104</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
       <c r="I32" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="K32" s="18">
         <v>0.3</v>
@@ -3244,20 +3170,17 @@
       <c r="L32" s="13">
         <v>12</v>
       </c>
-      <c r="M32" s="16">
-        <v>0.7</v>
-      </c>
-      <c r="N32" s="16">
-        <v>0.7</v>
-      </c>
-      <c r="O32" s="31"/>
-      <c r="P32" s="28"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="32"/>
-    </row>
-    <row r="33" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M32" s="46">
+        <v>1</v>
+      </c>
+      <c r="N32" s="31"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="32"/>
+    </row>
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B33" s="26" t="s">
         <v>106</v>
@@ -3269,10 +3192,10 @@
         <v>108</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
@@ -3284,16 +3207,17 @@
       <c r="L33" s="13">
         <v>12</v>
       </c>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
+      <c r="M33" s="46">
+        <v>1</v>
+      </c>
+      <c r="N33" s="10"/>
       <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
+      <c r="P33" s="11"/>
       <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-    </row>
-    <row r="34" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B34" s="26" t="s">
         <v>106</v>
@@ -3305,10 +3229,10 @@
         <v>111</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
@@ -3320,18 +3244,17 @@
       <c r="L34" s="13">
         <v>12</v>
       </c>
-      <c r="M34" s="16"/>
-      <c r="N34" s="16">
-        <v>1</v>
-      </c>
+      <c r="M34" s="46">
+        <v>1</v>
+      </c>
+      <c r="N34" s="10"/>
       <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
+      <c r="P34" s="11"/>
       <c r="Q34" s="11"/>
-      <c r="R34" s="11"/>
-    </row>
-    <row r="35" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B35" s="26" t="s">
         <v>113</v>
@@ -3343,10 +3266,10 @@
         <v>115</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
@@ -3358,18 +3281,17 @@
       <c r="L35" s="13">
         <v>12</v>
       </c>
-      <c r="M35" s="16"/>
-      <c r="N35" s="16">
-        <v>1</v>
-      </c>
+      <c r="M35" s="46">
+        <v>1</v>
+      </c>
+      <c r="N35" s="10"/>
       <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
+      <c r="P35" s="11"/>
       <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
-    </row>
-    <row r="36" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B36" s="26" t="s">
         <v>113</v>
@@ -3381,10 +3303,10 @@
         <v>118</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
@@ -3396,18 +3318,17 @@
       <c r="L36" s="13">
         <v>12</v>
       </c>
-      <c r="M36" s="16"/>
-      <c r="N36" s="16">
-        <v>1</v>
-      </c>
+      <c r="M36" s="46">
+        <v>1</v>
+      </c>
+      <c r="N36" s="10"/>
       <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
+      <c r="P36" s="11"/>
       <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-    </row>
-    <row r="37" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B37" s="26" t="s">
         <v>113</v>
@@ -3419,10 +3340,10 @@
         <v>121</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
@@ -3434,18 +3355,17 @@
       <c r="L37" s="13">
         <v>12</v>
       </c>
-      <c r="M37" s="16"/>
-      <c r="N37" s="16">
-        <v>1</v>
-      </c>
+      <c r="M37" s="46">
+        <v>1</v>
+      </c>
+      <c r="N37" s="10"/>
       <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
+      <c r="P37" s="11"/>
       <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-    </row>
-    <row r="38" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B38" s="26" t="s">
         <v>123</v>
@@ -3457,10 +3377,10 @@
         <v>125</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
@@ -3472,20 +3392,17 @@
       <c r="L38" s="13">
         <v>12</v>
       </c>
-      <c r="M38" s="16">
-        <v>1</v>
-      </c>
-      <c r="N38" s="16">
-        <v>1</v>
-      </c>
+      <c r="M38" s="46">
+        <v>1</v>
+      </c>
+      <c r="N38" s="10"/>
       <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
+      <c r="P38" s="11"/>
       <c r="Q38" s="11"/>
-      <c r="R38" s="11"/>
-    </row>
-    <row r="39" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B39" s="26" t="s">
         <v>123</v>
@@ -3497,10 +3414,10 @@
         <v>128</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
@@ -3512,20 +3429,17 @@
       <c r="L39" s="13">
         <v>12</v>
       </c>
-      <c r="M39" s="16">
-        <v>1</v>
-      </c>
-      <c r="N39" s="16">
-        <v>1</v>
-      </c>
+      <c r="M39" s="46">
+        <v>1</v>
+      </c>
+      <c r="N39" s="10"/>
       <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
+      <c r="P39" s="11"/>
       <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
-    </row>
-    <row r="40" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B40" s="26" t="s">
         <v>130</v>
@@ -3537,18 +3451,18 @@
         <v>132</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K40" s="18">
         <v>0.25</v>
@@ -3556,20 +3470,17 @@
       <c r="L40" s="13">
         <v>12</v>
       </c>
-      <c r="M40" s="16">
-        <v>1</v>
-      </c>
-      <c r="N40" s="16">
-        <v>2</v>
-      </c>
+      <c r="M40" s="46">
+        <v>1</v>
+      </c>
+      <c r="N40" s="10"/>
       <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
+      <c r="P40" s="11"/>
       <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-    </row>
-    <row r="41" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B41" s="26" t="s">
         <v>134</v>
@@ -3581,18 +3492,18 @@
         <v>136</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G41" s="12"/>
       <c r="H41" s="33"/>
       <c r="I41" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="K41" s="18">
         <v>0.25</v>
@@ -3600,20 +3511,17 @@
       <c r="L41" s="13">
         <v>12</v>
       </c>
-      <c r="M41" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="N41" s="16">
-        <v>2</v>
-      </c>
+      <c r="M41" s="46">
+        <v>1</v>
+      </c>
+      <c r="N41" s="10"/>
       <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
+      <c r="P41" s="11"/>
       <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-    </row>
-    <row r="42" spans="1:18" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:17" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B42" s="26" t="s">
         <v>134</v>
@@ -3625,18 +3533,18 @@
         <v>139</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G42" s="12"/>
       <c r="H42" s="33"/>
       <c r="I42" s="12" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="K42" s="18">
         <v>0.25</v>
@@ -3644,20 +3552,17 @@
       <c r="L42" s="13">
         <v>12</v>
       </c>
-      <c r="M42" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="N42" s="16">
-        <v>2</v>
-      </c>
+      <c r="M42" s="46">
+        <v>1</v>
+      </c>
+      <c r="N42" s="10"/>
       <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
+      <c r="P42" s="11"/>
       <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-    </row>
-    <row r="43" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B43" s="26" t="s">
         <v>134</v>
@@ -3669,10 +3574,10 @@
         <v>142</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
@@ -3684,18 +3589,17 @@
       <c r="L43" s="13">
         <v>12</v>
       </c>
-      <c r="M43" s="16"/>
-      <c r="N43" s="16">
-        <v>1</v>
-      </c>
+      <c r="M43" s="46">
+        <v>1</v>
+      </c>
+      <c r="N43" s="10"/>
       <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
+      <c r="P43" s="11"/>
       <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
-    </row>
-    <row r="44" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B44" s="26" t="s">
         <v>134</v>
@@ -3707,10 +3611,10 @@
         <v>145</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
@@ -3722,18 +3626,17 @@
       <c r="L44" s="13">
         <v>12</v>
       </c>
-      <c r="M44" s="16"/>
-      <c r="N44" s="16">
-        <v>1</v>
-      </c>
+      <c r="M44" s="46">
+        <v>1</v>
+      </c>
+      <c r="N44" s="10"/>
       <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
+      <c r="P44" s="11"/>
       <c r="Q44" s="11"/>
-      <c r="R44" s="11"/>
-    </row>
-    <row r="45" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B45" s="26" t="s">
         <v>134</v>
@@ -3745,18 +3648,18 @@
         <v>148</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
       <c r="I45" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="J45" s="12" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="K45" s="18">
         <v>0.7</v>
@@ -3764,20 +3667,17 @@
       <c r="L45" s="13">
         <v>12</v>
       </c>
-      <c r="M45" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="N45" s="16">
-        <v>2</v>
-      </c>
+      <c r="M45" s="46">
+        <v>1</v>
+      </c>
+      <c r="N45" s="10"/>
       <c r="O45" s="10"/>
-      <c r="P45" s="10"/>
+      <c r="P45" s="11"/>
       <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-    </row>
-    <row r="46" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B46" s="26" t="s">
         <v>134</v>
@@ -3789,18 +3689,18 @@
         <v>151</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
       <c r="I46" s="12" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="J46" s="12" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="K46" s="20">
         <v>0.7</v>
@@ -3808,20 +3708,17 @@
       <c r="L46" s="13">
         <v>12</v>
       </c>
-      <c r="M46" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="N46" s="16">
-        <v>2</v>
-      </c>
+      <c r="M46" s="46">
+        <v>1</v>
+      </c>
+      <c r="N46" s="10"/>
       <c r="O46" s="10"/>
-      <c r="P46" s="10"/>
+      <c r="P46" s="11"/>
       <c r="Q46" s="11"/>
-      <c r="R46" s="11"/>
-    </row>
-    <row r="47" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B47" s="26" t="s">
         <v>134</v>
@@ -3833,10 +3730,10 @@
         <v>154</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
@@ -3848,18 +3745,17 @@
       <c r="L47" s="13">
         <v>12</v>
       </c>
-      <c r="M47" s="16"/>
-      <c r="N47" s="16">
-        <v>1</v>
-      </c>
+      <c r="M47" s="46">
+        <v>1</v>
+      </c>
+      <c r="N47" s="10"/>
       <c r="O47" s="10"/>
-      <c r="P47" s="10"/>
+      <c r="P47" s="11"/>
       <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
-    </row>
-    <row r="48" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B48" s="26" t="s">
         <v>134</v>
@@ -3871,18 +3767,18 @@
         <v>157</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
       <c r="I48" s="12" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J48" s="12" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="K48" s="18">
         <v>0.2</v>
@@ -3890,20 +3786,17 @@
       <c r="L48" s="13">
         <v>12</v>
       </c>
-      <c r="M48" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="N48" s="16">
-        <v>2</v>
-      </c>
+      <c r="M48" s="46">
+        <v>1</v>
+      </c>
+      <c r="N48" s="10"/>
       <c r="O48" s="10"/>
-      <c r="P48" s="10"/>
+      <c r="P48" s="11"/>
       <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
-    </row>
-    <row r="49" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B49" s="26" t="s">
         <v>134</v>
@@ -3915,18 +3808,18 @@
         <v>160</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
       <c r="I49" s="12" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="J49" s="12" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K49" s="18">
         <v>0.3</v>
@@ -3934,20 +3827,17 @@
       <c r="L49" s="13">
         <v>12</v>
       </c>
-      <c r="M49" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="N49" s="16">
-        <v>2</v>
-      </c>
+      <c r="M49" s="46">
+        <v>1</v>
+      </c>
+      <c r="N49" s="10"/>
       <c r="O49" s="10"/>
-      <c r="P49" s="10"/>
+      <c r="P49" s="11"/>
       <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-    </row>
-    <row r="50" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B50" s="26" t="s">
         <v>134</v>
@@ -3959,37 +3849,34 @@
         <v>163</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G50" s="12"/>
       <c r="H50" s="12"/>
       <c r="I50" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="J50" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="K50" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="J50" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="K50" s="18" t="s">
-        <v>360</v>
-      </c>
       <c r="L50" s="13">
         <v>12</v>
       </c>
-      <c r="M50" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="N50" s="16">
-        <v>1</v>
-      </c>
+      <c r="M50" s="46">
+        <v>1</v>
+      </c>
+      <c r="N50" s="10"/>
       <c r="O50" s="10"/>
-      <c r="P50" s="10"/>
+      <c r="P50" s="11"/>
       <c r="Q50" s="11"/>
-      <c r="R50" s="11"/>
-    </row>
-    <row r="51" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="12" t="s">
         <v>51</v>
       </c>
@@ -4003,10 +3890,10 @@
         <v>167</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G51" s="12"/>
       <c r="H51" s="12"/>
@@ -4018,16 +3905,15 @@
       <c r="L51" s="13">
         <v>12</v>
       </c>
-      <c r="M51" s="16"/>
-      <c r="N51" s="16">
-        <v>1</v>
-      </c>
+      <c r="M51" s="46">
+        <v>1</v>
+      </c>
+      <c r="N51" s="10"/>
       <c r="O51" s="10"/>
-      <c r="P51" s="10"/>
+      <c r="P51" s="11"/>
       <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
-    </row>
-    <row r="52" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
         <v>51</v>
       </c>
@@ -4041,18 +3927,18 @@
         <v>170</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G52" s="12"/>
       <c r="H52" s="12"/>
       <c r="I52" s="12" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="J52" s="12" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="K52" s="18">
         <v>0.9</v>
@@ -4060,20 +3946,17 @@
       <c r="L52" s="13">
         <v>12</v>
       </c>
-      <c r="M52" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="N52" s="16">
-        <v>1</v>
-      </c>
+      <c r="M52" s="46">
+        <v>1</v>
+      </c>
+      <c r="N52" s="10"/>
       <c r="O52" s="10"/>
-      <c r="P52" s="10"/>
+      <c r="P52" s="11"/>
       <c r="Q52" s="11"/>
-      <c r="R52" s="11"/>
-    </row>
-    <row r="53" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B53" s="26" t="s">
         <v>172</v>
@@ -4085,39 +3968,36 @@
         <v>174</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G53" s="12"/>
       <c r="H53" s="12"/>
       <c r="I53" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="J53" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="K53" s="18" t="s">
         <v>370</v>
       </c>
-      <c r="J53" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="K53" s="18" t="s">
-        <v>372</v>
-      </c>
       <c r="L53" s="13">
         <v>12</v>
       </c>
-      <c r="M53" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="N53" s="16">
-        <v>2</v>
-      </c>
+      <c r="M53" s="46">
+        <v>1</v>
+      </c>
+      <c r="N53" s="10"/>
       <c r="O53" s="10"/>
-      <c r="P53" s="10"/>
+      <c r="P53" s="11"/>
       <c r="Q53" s="11"/>
-      <c r="R53" s="11"/>
-    </row>
-    <row r="54" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B54" s="26" t="s">
         <v>172</v>
@@ -4129,39 +4009,36 @@
         <v>177</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
       <c r="I54" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="J54" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="K54" s="18" t="s">
         <v>374</v>
       </c>
-      <c r="J54" s="12" t="s">
-        <v>375</v>
-      </c>
-      <c r="K54" s="18" t="s">
-        <v>376</v>
-      </c>
       <c r="L54" s="13">
         <v>12</v>
       </c>
-      <c r="M54" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="N54" s="16">
-        <v>2</v>
-      </c>
+      <c r="M54" s="46">
+        <v>1</v>
+      </c>
+      <c r="N54" s="10"/>
       <c r="O54" s="10"/>
-      <c r="P54" s="10"/>
+      <c r="P54" s="11"/>
       <c r="Q54" s="11"/>
-      <c r="R54" s="11"/>
-    </row>
-    <row r="55" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B55" s="26" t="s">
         <v>172</v>
@@ -4173,39 +4050,36 @@
         <v>180</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G55" s="12"/>
       <c r="H55" s="12"/>
       <c r="I55" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="J55" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="K55" s="18" t="s">
         <v>378</v>
       </c>
-      <c r="J55" s="12" t="s">
-        <v>379</v>
-      </c>
-      <c r="K55" s="18" t="s">
-        <v>380</v>
-      </c>
       <c r="L55" s="13">
         <v>12</v>
       </c>
-      <c r="M55" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="N55" s="16">
-        <v>2</v>
-      </c>
+      <c r="M55" s="46">
+        <v>1</v>
+      </c>
+      <c r="N55" s="10"/>
       <c r="O55" s="10"/>
-      <c r="P55" s="10"/>
+      <c r="P55" s="11"/>
       <c r="Q55" s="11"/>
-      <c r="R55" s="11"/>
-    </row>
-    <row r="56" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B56" s="26" t="s">
         <v>182</v>
@@ -4217,18 +4091,18 @@
         <v>184</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
       <c r="I56" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J56" s="12" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K56" s="18">
         <v>0.3</v>
@@ -4236,20 +4110,17 @@
       <c r="L56" s="13">
         <v>12</v>
       </c>
-      <c r="M56" s="16">
-        <v>1</v>
-      </c>
-      <c r="N56" s="16">
-        <v>2</v>
-      </c>
+      <c r="M56" s="46">
+        <v>1</v>
+      </c>
+      <c r="N56" s="10"/>
       <c r="O56" s="10"/>
-      <c r="P56" s="10"/>
+      <c r="P56" s="11"/>
       <c r="Q56" s="11"/>
-      <c r="R56" s="11"/>
-    </row>
-    <row r="57" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B57" s="26" t="s">
         <v>182</v>
@@ -4261,33 +4132,30 @@
         <v>187</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
       <c r="K57" s="15" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L57" s="13">
         <v>12</v>
       </c>
-      <c r="M57" s="16"/>
-      <c r="N57" s="16">
-        <v>1</v>
-      </c>
+      <c r="M57" s="46"/>
+      <c r="N57" s="10"/>
       <c r="O57" s="10"/>
-      <c r="P57" s="10"/>
+      <c r="P57" s="11"/>
       <c r="Q57" s="11"/>
-      <c r="R57" s="11"/>
-    </row>
-    <row r="58" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B58" s="26" t="s">
         <v>182</v>
@@ -4299,18 +4167,18 @@
         <v>167</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F58" s="22" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
       <c r="I58" s="12" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="J58" s="12" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="K58" s="15">
         <v>0.85</v>
@@ -4318,20 +4186,17 @@
       <c r="L58" s="13">
         <v>12</v>
       </c>
-      <c r="M58" s="16">
-        <v>1</v>
-      </c>
-      <c r="N58" s="16">
-        <v>2</v>
-      </c>
+      <c r="M58" s="46">
+        <v>1</v>
+      </c>
+      <c r="N58" s="10"/>
       <c r="O58" s="10"/>
-      <c r="P58" s="10"/>
+      <c r="P58" s="11"/>
       <c r="Q58" s="11"/>
-      <c r="R58" s="11"/>
-    </row>
-    <row r="59" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B59" s="26" t="s">
         <v>182</v>
@@ -4343,10 +4208,10 @@
         <v>192</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
@@ -4358,20 +4223,17 @@
       <c r="L59" s="13">
         <v>12</v>
       </c>
-      <c r="M59" s="16">
-        <v>1</v>
-      </c>
-      <c r="N59" s="16">
-        <v>2</v>
-      </c>
+      <c r="M59" s="46">
+        <v>1</v>
+      </c>
+      <c r="N59" s="10"/>
       <c r="O59" s="10"/>
-      <c r="P59" s="10"/>
+      <c r="P59" s="11"/>
       <c r="Q59" s="11"/>
-      <c r="R59" s="11"/>
-    </row>
-    <row r="60" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B60" s="26" t="s">
         <v>182</v>
@@ -4383,10 +4245,10 @@
         <v>195</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
@@ -4398,20 +4260,17 @@
       <c r="L60" s="13">
         <v>12</v>
       </c>
-      <c r="M60" s="16">
-        <v>1</v>
-      </c>
-      <c r="N60" s="16">
-        <v>2</v>
-      </c>
+      <c r="M60" s="46">
+        <v>1</v>
+      </c>
+      <c r="N60" s="10"/>
       <c r="O60" s="10"/>
-      <c r="P60" s="10"/>
+      <c r="P60" s="11"/>
       <c r="Q60" s="11"/>
-      <c r="R60" s="11"/>
-    </row>
-    <row r="61" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B61" s="26" t="s">
         <v>182</v>
@@ -4423,18 +4282,18 @@
         <v>198</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="G61" s="12"/>
       <c r="H61" s="12"/>
       <c r="I61" s="12" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="J61" s="12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="K61" s="34">
         <v>1</v>
@@ -4442,20 +4301,17 @@
       <c r="L61" s="13">
         <v>12</v>
       </c>
-      <c r="M61" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="N61" s="16">
-        <v>1</v>
-      </c>
+      <c r="M61" s="46">
+        <v>1</v>
+      </c>
+      <c r="N61" s="10"/>
       <c r="O61" s="10"/>
-      <c r="P61" s="10"/>
+      <c r="P61" s="11"/>
       <c r="Q61" s="11"/>
-      <c r="R61" s="11"/>
-    </row>
-    <row r="62" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:17" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B62" s="26" t="s">
         <v>182</v>
@@ -4467,18 +4323,18 @@
         <v>201</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G62" s="12"/>
       <c r="H62" s="12"/>
       <c r="I62" s="12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J62" s="12" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="K62" s="18">
         <v>0.95</v>
@@ -4486,18 +4342,15 @@
       <c r="L62" s="13">
         <v>12</v>
       </c>
-      <c r="M62" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="N62" s="16">
-        <v>1</v>
-      </c>
+      <c r="M62" s="46">
+        <v>1</v>
+      </c>
+      <c r="N62" s="10"/>
       <c r="O62" s="10"/>
-      <c r="P62" s="10"/>
+      <c r="P62" s="11"/>
       <c r="Q62" s="11"/>
-      <c r="R62" s="11"/>
-    </row>
-    <row r="63" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="19"/>
       <c r="B63" s="19"/>
       <c r="C63" s="19"/>
@@ -4511,13 +4364,12 @@
       <c r="K63" s="36"/>
       <c r="L63" s="35"/>
       <c r="M63" s="29"/>
-      <c r="N63" s="29"/>
+      <c r="N63" s="31"/>
       <c r="O63" s="31"/>
-      <c r="P63" s="31"/>
-      <c r="Q63" s="29"/>
-      <c r="R63" s="30"/>
-    </row>
-    <row r="64" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P63" s="29"/>
+      <c r="Q63" s="30"/>
+    </row>
+    <row r="64" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="19"/>
       <c r="B64" s="19"/>
       <c r="C64" s="19"/>
@@ -4531,13 +4383,12 @@
       <c r="K64" s="36"/>
       <c r="L64" s="35"/>
       <c r="M64" s="29"/>
-      <c r="N64" s="29"/>
+      <c r="N64" s="31"/>
       <c r="O64" s="31"/>
-      <c r="P64" s="31"/>
-      <c r="Q64" s="29"/>
-      <c r="R64" s="30"/>
-    </row>
-    <row r="65" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P64" s="29"/>
+      <c r="Q64" s="30"/>
+    </row>
+    <row r="65" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="19"/>
       <c r="B65" s="19"/>
       <c r="C65" s="19"/>
@@ -4551,15 +4402,14 @@
       <c r="K65" s="36"/>
       <c r="L65" s="35"/>
       <c r="M65" s="29"/>
-      <c r="N65" s="29"/>
-      <c r="O65" s="37"/>
-      <c r="P65" s="31"/>
-      <c r="Q65" s="29"/>
-      <c r="R65" s="28"/>
+      <c r="N65" s="37"/>
+      <c r="O65" s="31"/>
+      <c r="P65" s="29"/>
+      <c r="Q65" s="28"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M1:N1048576">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="M1:M1048576">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
finished tunning the naive runs
</commit_message>
<xml_diff>
--- a/ssp_modeling/scenario_mapping/ssp_morocco_transformation_cw.xlsx
+++ b/ssp_modeling/scenario_mapping/ssp_morocco_transformation_cw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Documents/sisepuede_modeling/ssp_morocco/ssp_modeling/scenario_mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDB247D-01BB-B94C-BDF8-E60C36F7A3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4CF85F-1717-8E42-8429-E0807712519D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1916,7 +1916,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>